<commit_message>
New imports after fixing blank line detection
</commit_message>
<xml_diff>
--- a/data/xls/2011-03-01/20110601-EERR8-repweb-Oct10-Mar11-Smith-Nephew.xlsx
+++ b/data/xls/2011-03-01/20110601-EERR8-repweb-Oct10-Mar11-Smith-Nephew.xlsx
@@ -1,175 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="23117"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="15" windowWidth="18960" windowHeight="11325"/>
+    <workbookView xWindow="120" yWindow="20" windowWidth="18960" windowHeight="11320"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve">Summary of Events Sponsored by Member Companies</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve">Reporting Period April - September 2010</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve">Company Name:               Smith &amp; Nephew Pty. Ltd.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve">Number of events held:                             2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve">Month:                                               Mar-11</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve">Description of function </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="9"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve">including</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve">  duration of educational content delivered</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve">Venue</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve">Professional
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve">status of attendees</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve">Hospitality provided</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve">Total cost of hospitality</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve">Number of attendees
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve">– number only</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve">Total cost of function</t>
-    </r>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <r>
       <rPr>
@@ -208,7 +58,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
       </rPr>
-      <t xml:space="preserve">April 2011. Smith &amp; Nephew Pty. Ltd. contributed to the sponsorship of the event via trade display attendance. The event was organised by the Australasian College of Phlebology Smith &amp; Nephew Pty. Ltd. was not responsible for inviting the attendees or organising the educational content, the hospitality, accommodation or travel. Four day program. Duration of educational content delivered: 28 hours.</t>
+      <t>April 2011. Smith &amp; Nephew Pty. Ltd. contributed to the sponsorship of the event via trade display attendance. The event was organised by the Australasian College of Phlebology Smith &amp; Nephew Pty. Ltd. was not responsible for inviting the attendees or organising the educational content, the hospitality, accommodation or travel. Four day program. Duration of educational content delivered: 28 hours.</t>
     </r>
   </si>
   <si>
@@ -225,7 +75,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
       </rPr>
-      <t xml:space="preserve">Melbourne</t>
+      <t>Melbourne</t>
     </r>
   </si>
   <si>
@@ -242,34 +92,34 @@
         <sz val="10"/>
         <rFont val="Arial"/>
       </rPr>
-      <t xml:space="preserve">Surgeons, Phlebologists</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve">No</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve">N/A</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve">150</t>
+      <t>Surgeons, Phlebologists</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>No</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>N/A</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>150</t>
     </r>
   </si>
   <si>
@@ -310,7 +160,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
       </rPr>
-      <t xml:space="preserve">costs of doing so.</t>
+      <t>costs of doing so.</t>
     </r>
   </si>
   <si>
@@ -359,7 +209,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
       </rPr>
-      <t xml:space="preserve">2 day program. Duration of educational content delivered: 14 hours.</t>
+      <t>2 day program. Duration of educational content delivered: 14 hours.</t>
     </r>
   </si>
   <si>
@@ -384,16 +234,16 @@
         <sz val="10"/>
         <rFont val="Arial"/>
       </rPr>
-      <t xml:space="preserve">Education Block</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve">180</t>
+      <t>Education Block</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>180</t>
     </r>
   </si>
   <si>
@@ -434,21 +284,126 @@
         <sz val="10"/>
         <rFont val="Arial"/>
       </rPr>
-      <t xml:space="preserve">costs of doing so.</t>
+      <t>costs of doing so.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>Description of function including duration of educational content delivered</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>Venue (Including suburb &amp; postcode)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>Professional Status of attendees</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>Hospitality Provided</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">Total Cost of
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>Hospitality</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">Number of confirmed
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>attendees</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">Total Cost of
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>Function</t>
     </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
-      <color rgb="#000000"/>
+      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
     </font>
   </fonts>
   <fills count="4">
@@ -465,7 +420,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF99CC00"/>
+        <fgColor rgb="FFD6E3BB"/>
       </patternFill>
     </fill>
   </fills>
@@ -496,18 +451,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fillId="2" borderId="0" fontId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fillId="3" borderId="1" fontId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fillId="2" borderId="1" fontId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fillId="2" borderId="1" fontId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -802,156 +760,99 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:O1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" customWidth="1" width="28"/>
-    <col min="2" max="2" customWidth="1" width="19.111111"/>
-    <col min="3" max="3" customWidth="1" width="20"/>
-    <col min="4" max="4" customWidth="1" width="19.333333"/>
-    <col min="5" max="5" customWidth="1" width="18.222222"/>
-    <col min="6" max="6" customWidth="1" width="21.777778"/>
-    <col min="7" max="7" customWidth="1" width="19.333333"/>
-    <col min="8" max="8" customWidth="1" width="2.666667"/>
+    <col min="1" max="1" width="28" customWidth="1"/>
+    <col min="2" max="2" width="19.1640625" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" customWidth="1"/>
+    <col min="5" max="5" width="18.1640625" customWidth="1"/>
+    <col min="6" max="6" width="21.83203125" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14" customHeight="1">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:7" ht="38" customHeight="1">
+      <c r="A1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="308" customHeight="1">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0"/>
-      <c r="C1" s="0"/>
-      <c r="D1" s="0"/>
-      <c r="E1" s="0"/>
-      <c r="F1" s="0"/>
-      <c r="G1" s="0"/>
-      <c r="H1" s="0"/>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" ht="14" customHeight="1">
-      <c r="A2" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0"/>
-      <c r="C2" s="0"/>
-      <c r="D2" s="0"/>
-      <c r="E2" s="0"/>
-      <c r="F2" s="0"/>
-      <c r="G2" s="0"/>
-      <c r="H2" s="0"/>
-    </row>
-    <row r="3" spans="1:8" ht="14" customHeight="1">
-      <c r="A3" s="0" t="s">
+    <row r="3" spans="1:7" ht="299" customHeight="1">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="0"/>
-      <c r="C3" s="0"/>
-      <c r="D3" s="0"/>
-      <c r="E3" s="0"/>
-      <c r="F3" s="0"/>
-      <c r="G3" s="0"/>
-      <c r="H3" s="0"/>
-    </row>
-    <row r="4" spans="1:8" ht="14" customHeight="1">
-      <c r="A4" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="0"/>
-      <c r="C4" s="0"/>
-      <c r="D4" s="0"/>
-      <c r="E4" s="0"/>
-      <c r="F4" s="0"/>
-      <c r="G4" s="0"/>
-      <c r="H4" s="0"/>
-    </row>
-    <row r="5" spans="1:8" ht="14" customHeight="1">
-      <c r="A5" s="0" t="s">
+      <c r="E3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="0"/>
-      <c r="C5" s="0"/>
-      <c r="D5" s="0"/>
-      <c r="E5" s="0"/>
-      <c r="F5" s="0"/>
-      <c r="G5" s="0"/>
-      <c r="H5" s="0"/>
-    </row>
-    <row r="6" spans="1:8" ht="46" customHeight="1">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="1" t="s">
+      <c r="F3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="0"/>
-    </row>
-    <row r="7" spans="1:8" ht="308" customHeight="1">
-      <c r="A7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" s="0"/>
-    </row>
-    <row r="8" spans="1:8" ht="299" customHeight="1">
-      <c r="A8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H8" s="0"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>